<commit_message>
Working version with KO indide. Need some more style tweeking.
</commit_message>
<xml_diff>
--- a/data/galilean.xlsx
+++ b/data/galilean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspace\EREZ\galilean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267A0E5E-848D-479A-9409-824EBFE03CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF0555B-02EC-402D-B0F9-6CCA14C57FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{478A9EFA-3F6C-41E7-929E-7486A48D12FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{478A9EFA-3F6C-41E7-929E-7486A48D12FC}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="pictures" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -537,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED8B9A2-89A4-435F-9481-E3CC8DAC7B93}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,10 +625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB7DD92-97E3-45E3-87DC-96A5E8516544}">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,10 +773,14 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -799,7 +804,9 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -898,12 +905,28 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="A15" s="6">
+        <v>21</v>
+      </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1724,7 +1747,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1777,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="2">
-        <v>2000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>